<commit_message>
Add four new sites
</commit_message>
<xml_diff>
--- a/overall_stats.xlsx
+++ b/overall_stats.xlsx
@@ -1,30 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ricerca\Altro\AssistiveGenerativeAI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ricerca\Altre\AssistiveGenerativeAI\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8639F03-6F27-4044-8CE2-0891086B29A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23280" windowHeight="11385"/>
+    <workbookView xWindow="4230" yWindow="330" windowWidth="24075" windowHeight="14400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
   <si>
     <t>Univaq</t>
   </si>
@@ -70,11 +82,23 @@
   <si>
     <t>Questions</t>
   </si>
+  <si>
+    <t>Amazon</t>
+  </si>
+  <si>
+    <t>Google</t>
+  </si>
+  <si>
+    <t>Weather.com</t>
+  </si>
+  <si>
+    <t>Reddit</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="\(0\%\)"/>
   </numFmts>
@@ -200,26 +224,29 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -277,7 +304,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -340,9 +366,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Foglio1!$A$3:$A$11</c:f>
+              <c:f>Foglio1!$A$3:$A$15</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>Univaq</c:v>
                 </c:pt>
@@ -368,6 +394,18 @@
                   <c:v>Youtube</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>Amazon</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Google</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Weather.com</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Reddit</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>Cambridge Dictionary</c:v>
                 </c:pt>
               </c:strCache>
@@ -375,10 +413,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Foglio1!$C$3:$C$11</c:f>
+              <c:f>Foglio1!$C$3:$C$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>4</c:v>
                 </c:pt>
@@ -404,6 +442,18 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
@@ -444,10 +494,10 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Foglio1!$E$3:$E$11</c:f>
+              <c:f>Foglio1!$E$3:$E$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -473,6 +523,18 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -510,10 +572,10 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Foglio1!$G$3:$G$11</c:f>
+              <c:f>Foglio1!$G$3:$G$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -539,6 +601,18 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -755,7 +829,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -818,9 +891,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Foglio1!$A$3:$A$11</c:f>
+              <c:f>Foglio1!$A$3:$A$15</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>Univaq</c:v>
                 </c:pt>
@@ -846,6 +919,18 @@
                   <c:v>Youtube</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>Amazon</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Google</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Weather.com</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Reddit</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>Cambridge Dictionary</c:v>
                 </c:pt>
               </c:strCache>
@@ -853,10 +938,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Foglio1!$I$3:$I$11</c:f>
+              <c:f>Foglio1!$I$3:$I$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>4</c:v>
                 </c:pt>
@@ -882,6 +967,18 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
@@ -922,10 +1019,10 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Foglio1!$K$3:$K$11</c:f>
+              <c:f>Foglio1!$K$3:$K$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -951,6 +1048,18 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
@@ -978,7 +1087,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent3"/>
+              <a:srgbClr val="C00000"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -1007,10 +1116,10 @@
           </c:dPt>
           <c:val>
             <c:numRef>
-              <c:f>Foglio1!$M$3:$M$11</c:f>
+              <c:f>Foglio1!$M$3:$M$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>2</c:v>
                 </c:pt>
@@ -1036,6 +1145,18 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -2308,18 +2429,24 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Grafico 1"/>
+        <xdr:cNvPr id="2" name="Grafico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2338,18 +2465,24 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Grafico 2"/>
+        <xdr:cNvPr id="3" name="Grafico 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2629,24 +2762,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B3:B11"/>
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.28515625" customWidth="1"/>
-    <col min="3" max="3" width="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="3" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="7" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="2" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="6" bestFit="1" customWidth="1"/>
@@ -2655,511 +2788,752 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1" t="s">
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B2" s="10"/>
-      <c r="C2" s="2" t="s">
+      <c r="B2" s="7"/>
+      <c r="C2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="7"/>
-      <c r="E2" s="2" t="s">
+      <c r="D2" s="10"/>
+      <c r="E2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="7"/>
-      <c r="G2" s="2" t="s">
+      <c r="F2" s="10"/>
+      <c r="G2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="7"/>
-      <c r="I2" s="2" t="s">
+      <c r="H2" s="10"/>
+      <c r="I2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="7"/>
-      <c r="K2" s="2" t="s">
+      <c r="J2" s="10"/>
+      <c r="K2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="7"/>
-      <c r="M2" s="2" t="s">
+      <c r="L2" s="10"/>
+      <c r="M2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="N2" s="2"/>
+      <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B3">
         <f>C3+E3+G3+I3+K3+M3</f>
         <v>12</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="2">
         <v>4</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="3">
         <f>C3/($C3+$E3+$G3)*100</f>
         <v>66.666666666666657</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="2">
         <v>1</v>
       </c>
-      <c r="F3" s="5">
-        <f t="shared" ref="F3:F11" si="0">E3/($C3+$E3+$G3)*100</f>
+      <c r="F3" s="3">
+        <f t="shared" ref="F3:F15" si="0">E3/($C3+$E3+$G3)*100</f>
         <v>16.666666666666664</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="2">
         <v>1</v>
       </c>
-      <c r="H3" s="5">
-        <f t="shared" ref="H3:H11" si="1">G3/($C3+$E3+$G3)*100</f>
+      <c r="H3" s="3">
+        <f t="shared" ref="H3:H15" si="1">G3/($C3+$E3+$G3)*100</f>
         <v>16.666666666666664</v>
       </c>
-      <c r="I3" s="4">
+      <c r="I3" s="2">
         <v>4</v>
       </c>
-      <c r="J3" s="5">
+      <c r="J3" s="3">
         <f>I3/($I3+$K3+$M3)*100</f>
         <v>66.666666666666657</v>
       </c>
-      <c r="K3" s="4">
-        <v>0</v>
-      </c>
-      <c r="L3" s="5">
-        <f t="shared" ref="L3:L11" si="2">K3/($I3+$K3+$M3)*100</f>
-        <v>0</v>
-      </c>
-      <c r="M3" s="4">
+      <c r="K3" s="2">
+        <v>0</v>
+      </c>
+      <c r="L3" s="3">
+        <f t="shared" ref="L3:L15" si="2">K3/($I3+$K3+$M3)*100</f>
+        <v>0</v>
+      </c>
+      <c r="M3" s="2">
         <v>2</v>
       </c>
-      <c r="N3" s="6">
-        <f t="shared" ref="N3:N11" si="3">M3/($I3+$K3+$M3)*100</f>
+      <c r="N3" s="4">
+        <f t="shared" ref="N3:N15" si="3">M3/($I3+$K3+$M3)*100</f>
         <v>33.333333333333329</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="8">
-        <f t="shared" ref="B4:B11" si="4">C4+E4+G4+I4+K4+M4</f>
+      <c r="B4" s="5">
+        <f t="shared" ref="B4:B15" si="4">C4+E4+G4+I4+K4+M4</f>
         <v>7</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="2">
         <v>4</v>
       </c>
-      <c r="D4" s="5">
-        <f t="shared" ref="D4:D11" si="5">C4/($C4+$E4+$G4)*100</f>
+      <c r="D4" s="3">
+        <f t="shared" ref="D4:D15" si="5">C4/($C4+$E4+$G4)*100</f>
         <v>66.666666666666657</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="2">
         <v>2</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="3">
         <f t="shared" si="0"/>
         <v>33.333333333333329</v>
       </c>
-      <c r="G4" s="4">
-        <v>0</v>
-      </c>
-      <c r="H4" s="5">
+      <c r="G4" s="2">
+        <v>0</v>
+      </c>
+      <c r="H4" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I4" s="4">
+      <c r="I4" s="2">
         <v>1</v>
       </c>
-      <c r="J4" s="5">
-        <f t="shared" ref="J4:J11" si="6">I4/($I4+$K4+$M4)*100</f>
+      <c r="J4" s="3">
+        <f t="shared" ref="J4:J15" si="6">I4/($I4+$K4+$M4)*100</f>
         <v>100</v>
       </c>
-      <c r="K4" s="4">
-        <v>0</v>
-      </c>
-      <c r="L4" s="5">
+      <c r="K4" s="2">
+        <v>0</v>
+      </c>
+      <c r="L4" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M4" s="4">
-        <v>0</v>
-      </c>
-      <c r="N4" s="6">
+      <c r="M4" s="2">
+        <v>0</v>
+      </c>
+      <c r="N4" s="4">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5" s="5">
         <f t="shared" si="4"/>
         <v>5</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="2">
         <v>3</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="3">
         <f t="shared" si="5"/>
         <v>75</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="2">
         <v>1</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="3">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="G5" s="4">
-        <v>0</v>
-      </c>
-      <c r="H5" s="5">
+      <c r="G5" s="2">
+        <v>0</v>
+      </c>
+      <c r="H5" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I5" s="4">
+      <c r="I5" s="2">
         <v>1</v>
       </c>
-      <c r="J5" s="5">
+      <c r="J5" s="3">
         <f t="shared" si="6"/>
         <v>100</v>
       </c>
-      <c r="K5" s="4">
-        <v>0</v>
-      </c>
-      <c r="L5" s="5">
+      <c r="K5" s="2">
+        <v>0</v>
+      </c>
+      <c r="L5" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M5" s="4">
-        <v>0</v>
-      </c>
-      <c r="N5" s="6">
+      <c r="M5" s="2">
+        <v>0</v>
+      </c>
+      <c r="N5" s="4">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B6" s="5">
         <f t="shared" si="4"/>
         <v>8</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="2">
         <v>4</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="3">
         <f t="shared" si="5"/>
         <v>80</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="2">
         <v>1</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="3">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="G6" s="4">
-        <v>0</v>
-      </c>
-      <c r="H6" s="5">
+      <c r="G6" s="2">
+        <v>0</v>
+      </c>
+      <c r="H6" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I6" s="4">
+      <c r="I6" s="2">
         <v>2</v>
       </c>
-      <c r="J6" s="5">
+      <c r="J6" s="3">
         <f t="shared" si="6"/>
         <v>66.666666666666657</v>
       </c>
-      <c r="K6" s="4">
+      <c r="K6" s="2">
         <v>1</v>
       </c>
-      <c r="L6" s="5">
+      <c r="L6" s="3">
         <f t="shared" si="2"/>
         <v>33.333333333333329</v>
       </c>
-      <c r="M6" s="4">
-        <v>0</v>
-      </c>
-      <c r="N6" s="6">
+      <c r="M6" s="2">
+        <v>0</v>
+      </c>
+      <c r="N6" s="4">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="8">
+      <c r="B7" s="5">
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="2">
         <v>1</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="3">
         <f t="shared" si="5"/>
         <v>50</v>
       </c>
-      <c r="E7" s="4">
-        <v>0</v>
-      </c>
-      <c r="F7" s="5">
+      <c r="E7" s="2">
+        <v>0</v>
+      </c>
+      <c r="F7" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="2">
         <v>1</v>
       </c>
-      <c r="H7" s="5">
+      <c r="H7" s="3">
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="I7" s="4">
+      <c r="I7" s="2">
         <v>2</v>
       </c>
-      <c r="J7" s="5">
+      <c r="J7" s="3">
         <f t="shared" si="6"/>
         <v>100</v>
       </c>
-      <c r="K7" s="4">
-        <v>0</v>
-      </c>
-      <c r="L7" s="5">
+      <c r="K7" s="2">
+        <v>0</v>
+      </c>
+      <c r="L7" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M7" s="4">
-        <v>0</v>
-      </c>
-      <c r="N7" s="6">
+      <c r="M7" s="2">
+        <v>0</v>
+      </c>
+      <c r="N7" s="4">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="8">
+      <c r="B8" s="5">
         <f t="shared" si="4"/>
         <v>6</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="2">
         <v>2</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="3">
         <f t="shared" si="5"/>
         <v>66.666666666666657</v>
       </c>
-      <c r="E8" s="4">
-        <v>0</v>
-      </c>
-      <c r="F8" s="5">
+      <c r="E8" s="2">
+        <v>0</v>
+      </c>
+      <c r="F8" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="2">
         <v>1</v>
       </c>
-      <c r="H8" s="5">
+      <c r="H8" s="3">
         <f t="shared" si="1"/>
         <v>33.333333333333329</v>
       </c>
-      <c r="I8" s="4">
+      <c r="I8" s="2">
         <v>3</v>
       </c>
-      <c r="J8" s="5">
+      <c r="J8" s="3">
         <f t="shared" si="6"/>
         <v>100</v>
       </c>
-      <c r="K8" s="4">
-        <v>0</v>
-      </c>
-      <c r="L8" s="5">
+      <c r="K8" s="2">
+        <v>0</v>
+      </c>
+      <c r="L8" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M8" s="4">
-        <v>0</v>
-      </c>
-      <c r="N8" s="6">
+      <c r="M8" s="2">
+        <v>0</v>
+      </c>
+      <c r="N8" s="4">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B9" s="5">
         <f t="shared" si="4"/>
         <v>6</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="2">
         <v>2</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="3">
         <f t="shared" si="5"/>
         <v>66.666666666666657</v>
       </c>
-      <c r="E9" s="4">
-        <v>0</v>
-      </c>
-      <c r="F9" s="5">
+      <c r="E9" s="2">
+        <v>0</v>
+      </c>
+      <c r="F9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9" s="2">
         <v>1</v>
       </c>
-      <c r="H9" s="5">
+      <c r="H9" s="3">
         <f t="shared" si="1"/>
         <v>33.333333333333329</v>
       </c>
-      <c r="I9" s="4">
+      <c r="I9" s="2">
         <v>3</v>
       </c>
-      <c r="J9" s="5">
+      <c r="J9" s="3">
         <f t="shared" si="6"/>
         <v>100</v>
       </c>
-      <c r="K9" s="4">
-        <v>0</v>
-      </c>
-      <c r="L9" s="5">
+      <c r="K9" s="2">
+        <v>0</v>
+      </c>
+      <c r="L9" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M9" s="4">
-        <v>0</v>
-      </c>
-      <c r="N9" s="6">
+      <c r="M9" s="2">
+        <v>0</v>
+      </c>
+      <c r="N9" s="4">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="8">
+      <c r="B10" s="5">
         <f t="shared" si="4"/>
         <v>9</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="2">
         <v>4</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="3">
         <f t="shared" si="5"/>
         <v>80</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="2">
         <v>1</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="3">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="G10" s="4">
-        <v>0</v>
-      </c>
-      <c r="H10" s="5">
+      <c r="G10" s="2">
+        <v>0</v>
+      </c>
+      <c r="H10" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I10" s="4">
+      <c r="I10" s="2">
         <v>3</v>
       </c>
-      <c r="J10" s="5">
+      <c r="J10" s="3">
         <f t="shared" si="6"/>
         <v>75</v>
       </c>
-      <c r="K10" s="4">
+      <c r="K10" s="2">
         <v>1</v>
       </c>
-      <c r="L10" s="5">
+      <c r="L10" s="3">
         <f t="shared" si="2"/>
         <v>25</v>
       </c>
-      <c r="M10" s="4">
-        <v>0</v>
-      </c>
-      <c r="N10" s="6">
+      <c r="M10" s="2">
+        <v>0</v>
+      </c>
+      <c r="N10" s="4">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="5">
+        <f t="shared" si="4"/>
+        <v>15</v>
+      </c>
+      <c r="C11" s="2">
+        <v>1</v>
+      </c>
+      <c r="D11" s="3">
+        <f t="shared" si="5"/>
+        <v>100</v>
+      </c>
+      <c r="E11" s="2">
+        <v>0</v>
+      </c>
+      <c r="F11" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G11" s="2">
+        <v>0</v>
+      </c>
+      <c r="H11" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I11" s="2">
+        <v>10</v>
+      </c>
+      <c r="J11" s="3">
+        <f t="shared" si="6"/>
+        <v>71.428571428571431</v>
+      </c>
+      <c r="K11" s="2">
+        <v>3</v>
+      </c>
+      <c r="L11" s="3">
+        <f t="shared" si="2"/>
+        <v>21.428571428571427</v>
+      </c>
+      <c r="M11" s="2">
+        <v>1</v>
+      </c>
+      <c r="N11" s="4">
+        <f t="shared" si="3"/>
+        <v>7.1428571428571423</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="5">
+        <f t="shared" si="4"/>
+        <v>11</v>
+      </c>
+      <c r="C12" s="2">
+        <v>1</v>
+      </c>
+      <c r="D12" s="3">
+        <f t="shared" si="5"/>
+        <v>50</v>
+      </c>
+      <c r="E12" s="2">
+        <v>1</v>
+      </c>
+      <c r="F12" s="3">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="G12" s="2">
+        <v>0</v>
+      </c>
+      <c r="H12" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I12" s="2">
+        <v>4</v>
+      </c>
+      <c r="J12" s="3">
+        <f t="shared" si="6"/>
+        <v>44.444444444444443</v>
+      </c>
+      <c r="K12" s="2">
+        <v>1</v>
+      </c>
+      <c r="L12" s="3">
+        <f t="shared" si="2"/>
+        <v>11.111111111111111</v>
+      </c>
+      <c r="M12" s="2">
+        <v>4</v>
+      </c>
+      <c r="N12" s="4">
+        <f t="shared" si="3"/>
+        <v>44.444444444444443</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="5">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="C13" s="2">
+        <v>0</v>
+      </c>
+      <c r="D13" s="3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0</v>
+      </c>
+      <c r="F13" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G13" s="2">
+        <v>1</v>
+      </c>
+      <c r="H13" s="3">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="I13" s="2">
+        <v>0</v>
+      </c>
+      <c r="J13" s="3">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K13" s="2">
+        <v>2</v>
+      </c>
+      <c r="L13" s="3">
+        <f t="shared" si="2"/>
+        <v>50</v>
+      </c>
+      <c r="M13" s="2">
+        <v>2</v>
+      </c>
+      <c r="N13" s="4">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="5">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0</v>
+      </c>
+      <c r="D14" s="3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0</v>
+      </c>
+      <c r="F14" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G14" s="2">
+        <v>1</v>
+      </c>
+      <c r="H14" s="3">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="I14" s="2">
+        <v>1</v>
+      </c>
+      <c r="J14" s="3">
+        <f t="shared" si="6"/>
+        <v>25</v>
+      </c>
+      <c r="K14" s="2">
+        <v>0</v>
+      </c>
+      <c r="L14" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M14" s="2">
+        <v>3</v>
+      </c>
+      <c r="N14" s="4">
+        <f t="shared" si="3"/>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="8">
+      <c r="B15" s="5">
         <f t="shared" si="4"/>
         <v>7</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C15" s="2">
         <v>1</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D15" s="3">
         <f t="shared" si="5"/>
         <v>100</v>
       </c>
-      <c r="E11" s="4">
-        <v>0</v>
-      </c>
-      <c r="F11" s="5">
+      <c r="E15" s="2">
+        <v>0</v>
+      </c>
+      <c r="F15" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G11" s="4">
-        <v>0</v>
-      </c>
-      <c r="H11" s="5">
+      <c r="G15" s="2">
+        <v>0</v>
+      </c>
+      <c r="H15" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I11" s="4">
+      <c r="I15" s="2">
         <v>4</v>
       </c>
-      <c r="J11" s="5">
+      <c r="J15" s="3">
         <f t="shared" si="6"/>
         <v>66.666666666666657</v>
       </c>
-      <c r="K11" s="4">
+      <c r="K15" s="2">
         <v>2</v>
       </c>
-      <c r="L11" s="5">
+      <c r="L15" s="3">
         <f t="shared" si="2"/>
         <v>33.333333333333329</v>
       </c>
-      <c r="M11" s="4">
-        <v>0</v>
-      </c>
-      <c r="N11" s="6">
+      <c r="M15" s="2">
+        <v>0</v>
+      </c>
+      <c r="N15" s="4">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="11"/>
+      <c r="B16" s="11">
+        <f>SUM(B3:B15)</f>
+        <v>100</v>
+      </c>
+      <c r="C16" s="12">
+        <f>SUM(C3:C15)</f>
+        <v>27</v>
+      </c>
+      <c r="D16" s="13"/>
+      <c r="E16" s="12">
+        <f>SUM(E3:E15)</f>
+        <v>7</v>
+      </c>
+      <c r="F16" s="13"/>
+      <c r="G16" s="12">
+        <f>SUM(G3:G15)</f>
+        <v>6</v>
+      </c>
+      <c r="H16" s="13"/>
+      <c r="I16" s="12">
+        <f>SUM(I3:I15)</f>
+        <v>38</v>
+      </c>
+      <c r="J16" s="13"/>
+      <c r="K16" s="12">
+        <f>SUM(K3:K15)</f>
+        <v>10</v>
+      </c>
+      <c r="L16" s="13"/>
+      <c r="M16" s="12">
+        <f>SUM(M3:M15)</f>
+        <v>12</v>
+      </c>
+      <c r="N16" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>